<commit_message>
1. Goodlife code has added
2. Grouping in XMl file - done

3. Book service code FSC- done
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>9958592171</t>
   </si>
@@ -23,6 +24,12 @@
   </si>
   <si>
     <t>995859</t>
+  </si>
+  <si>
+    <t>Goodlife nonmem</t>
+  </si>
+  <si>
+    <t>Book service FSC</t>
   </si>
 </sst>
 </file>
@@ -365,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,6 +398,40 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel data changed for goodlife
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -17,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>9958592171</t>
-  </si>
-  <si>
     <t>8800996793</t>
   </si>
   <si>
@@ -30,6 +27,9 @@
   </si>
   <si>
     <t>Book service FSC</t>
+  </si>
+  <si>
+    <t>2537461015</t>
   </si>
 </sst>
 </file>
@@ -375,27 +375,27 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
@@ -411,7 +411,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,12 +421,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
All test case flow has update to date- 7 Jan
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>8800996793</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>2537461015</t>
+  </si>
+  <si>
+    <t>8800996794</t>
   </si>
 </sst>
 </file>
@@ -374,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,6 +401,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
     </row>
@@ -410,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Code is given by Pawan
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="2300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="2300"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
     <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId2"/>
     <sheet name="Book Service" sheetId="3" r:id="rId3"/>
+    <sheet name="My Profile" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -390,13 +391,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -462,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -477,4 +478,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>